<commit_message>
finished the design of dashboard, added edit profile page, and added some models
</commit_message>
<xml_diff>
--- a/Liam's_GanttChart.xlsx
+++ b/Liam's_GanttChart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\liams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BSIT3\327\liams_activity_log_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE164AD-9E66-4142-BF77-8EA9CEAF9A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C9D1E0-46ED-47F8-BCBE-9D03119C852C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6C8612AF-AC9F-47E5-97F5-BEE5B3F3935B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6C8612AF-AC9F-47E5-97F5-BEE5B3F3935B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Members:</t>
   </si>
@@ -75,12 +75,6 @@
     <t xml:space="preserve">Status </t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -102,40 +96,52 @@
     <t>Liam's Flavored Chicken Wing Activity Log System</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>2.1 Function requirements</t>
-  </si>
-  <si>
     <t>2. Analysis Description</t>
   </si>
   <si>
-    <t>2.2 Logical Model</t>
-  </si>
-  <si>
     <t>3. Created a design in FIGMA of Liam's System</t>
   </si>
   <si>
-    <t>3.1 Dashboard and User authentication pages</t>
-  </si>
-  <si>
-    <t>3.2 Activity Log and Feedback Pages</t>
-  </si>
-  <si>
-    <t>3.3 Leave and Branch Management Pages</t>
-  </si>
-  <si>
     <t>4. Implemented its pages to Django</t>
   </si>
   <si>
-    <t>4.1 User Authentication Pages</t>
-  </si>
-  <si>
     <t>In - Progress</t>
   </si>
   <si>
-    <t>5. UI design of Leave and Branch</t>
+    <t>Calimpong</t>
+  </si>
+  <si>
+    <t>Donaire</t>
+  </si>
+  <si>
+    <t>Gitgano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     2.1 Function requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     2.2 Logical Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     3.1 Dashboard and User authentication pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     3.2 Activity Log and Feedback Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     3.3 Leave and Branch Management Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     4.2 UI design of Leave and Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     4.3 UI design of Dashboard </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     4.1 UI design Login and Registration </t>
+  </si>
+  <si>
+    <t>5. Implementation of default accounts such as Admins and Super Admins</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -226,11 +232,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -257,6 +289,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,9 +313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -315,7 +353,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -421,7 +459,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -563,7 +601,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,26 +609,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEE28BF-3653-487B-ABAE-D8576A0DB2DF}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="5" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="69.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+    <col min="3" max="5" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="15"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="15"/>
       <c r="C2" s="3"/>
@@ -605,7 +643,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -622,9 +660,9 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -639,9 +677,9 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -656,9 +694,9 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -673,7 +711,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -688,7 +726,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -707,7 +745,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="5"/>
       <c r="C9" s="3" t="s">
@@ -724,7 +762,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="6"/>
       <c r="C10" s="3" t="s">
@@ -741,7 +779,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="7"/>
       <c r="C11" s="3" t="s">
@@ -758,7 +796,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -777,7 +815,7 @@
       <c r="L12" s="14"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
@@ -818,12 +856,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>16</v>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C14" s="11">
         <v>45534</v>
@@ -843,12 +881,12 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="C15" s="13">
         <v>45558</v>
@@ -868,12 +906,12 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="13">
         <v>45558</v>
@@ -893,12 +931,12 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C17" s="13">
         <v>45558</v>
@@ -918,12 +956,12 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>16</v>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="11">
         <v>45576</v>
@@ -943,12 +981,12 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="11">
         <v>45576</v>
@@ -963,19 +1001,19 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C20" s="11">
         <v>45576</v>
@@ -995,12 +1033,12 @@
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>14</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="11">
         <v>45576</v>
@@ -1020,12 +1058,12 @@
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>16</v>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="C22" s="11">
         <v>45598</v>
@@ -1034,7 +1072,7 @@
         <v>45599</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -1045,12 +1083,12 @@
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="C23" s="11">
         <v>45598</v>
@@ -1070,12 +1108,12 @@
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="C24" s="11">
         <v>45614</v>
@@ -1095,12 +1133,22 @@
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="18">
+        <v>45613</v>
+      </c>
+      <c r="D25" s="18">
+        <v>45617</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -1109,6 +1157,29 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="19">
+        <v>45618</v>
+      </c>
+      <c r="D26" s="20"/>
+      <c r="E26" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1122,15 +1193,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001570A2FF68DCA949B44B7843430634DD" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d492fbf2c015021d2019a9cb2628d99b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9ed737b4-88ac-4996-b253-4b3010066cf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="65370a0183c9b5c233b7f8b9de795d89" ns2:_="">
     <xsd:import namespace="9ed737b4-88ac-4996-b253-4b3010066cf9"/>
@@ -1274,6 +1336,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1281,14 +1352,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE939D89-B64E-4D9C-83A0-BE33138990E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D08AC5F-492E-4A0A-9218-240F32F41F20}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1306,6 +1369,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE939D89-B64E-4D9C-83A0-BE33138990E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF91549C-21D9-41B9-BD65-69654B49B349}">
   <ds:schemaRefs>

</xml_diff>